<commit_message>
25.10.21 Update to 01
</commit_message>
<xml_diff>
--- a/input_reference_tables/STIP Regions List.xlsx
+++ b/input_reference_tables/STIP Regions List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\25Q1_STIP\STIP_SCRIPTS\nys-stip-classification\input_reference_tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1D87589-CE72-4CF9-8E57-75E2DBBFC6E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D01698B-7861-4E18-89F4-1B60E8D9E37D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="2475" windowWidth="24240" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,17 +26,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="56">
-  <si>
-    <t>Code</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="57">
   <si>
     <t>NYSDOT Region</t>
   </si>
   <si>
-    <t>NYSDOT Region Name</t>
-  </si>
-  <si>
     <t>Counties</t>
   </si>
   <si>
@@ -194,6 +188,15 @@
   </si>
   <si>
     <t>index</t>
+  </si>
+  <si>
+    <t>Region</t>
+  </si>
+  <si>
+    <t>Region Code &amp; Name</t>
+  </si>
+  <si>
+    <t>Region Name</t>
   </si>
 </sst>
 </file>
@@ -560,7 +563,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:XFD1"/>
+      <selection pane="bottomLeft" activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -572,19 +575,19 @@
   <sheetData>
     <row r="1" spans="1:5" s="7" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="B1" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="7" t="s">
+      <c r="D1" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="E1" s="7" t="s">
         <v>1</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
@@ -592,16 +595,16 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
@@ -609,16 +612,16 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
@@ -626,16 +629,16 @@
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
@@ -643,16 +646,16 @@
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
@@ -660,16 +663,16 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="E6" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
@@ -677,16 +680,16 @@
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="E7" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
@@ -694,16 +697,16 @@
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="E8" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
@@ -711,16 +714,16 @@
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="E9" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
@@ -728,16 +731,16 @@
         <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="E10" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
@@ -745,16 +748,16 @@
         <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="E11" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
@@ -762,16 +765,16 @@
         <v>10</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="E12" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
@@ -779,16 +782,16 @@
         <v>11</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="E13" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1792,27 +1795,27 @@
   <sheetData>
     <row r="1" spans="1:5" ht="36" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>3</v>
-      </c>
       <c r="C1" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>51</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="34.200000000000003" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>8</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>10</v>
       </c>
       <c r="C2" s="6" t="e">
         <v>#VALUE!</v>
@@ -1826,10 +1829,10 @@
     </row>
     <row r="3" spans="1:5" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>12</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>14</v>
       </c>
       <c r="C3" s="6" t="e">
         <v>#VALUE!</v>
@@ -1843,10 +1846,10 @@
     </row>
     <row r="4" spans="1:5" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>16</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>18</v>
       </c>
       <c r="C4" s="6" t="e">
         <v>#VALUE!</v>
@@ -1860,10 +1863,10 @@
     </row>
     <row r="5" spans="1:5" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>20</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>22</v>
       </c>
       <c r="C5" s="6" t="e">
         <v>#VALUE!</v>
@@ -1877,10 +1880,10 @@
     </row>
     <row r="6" spans="1:5" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>24</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>26</v>
       </c>
       <c r="C6" s="6" t="e">
         <v>#VALUE!</v>
@@ -1894,10 +1897,10 @@
     </row>
     <row r="7" spans="1:5" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="5" t="s">
         <v>28</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>30</v>
       </c>
       <c r="C7" s="6" t="e">
         <v>#VALUE!</v>
@@ -1911,10 +1914,10 @@
     </row>
     <row r="8" spans="1:5" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="5" t="s">
         <v>32</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>34</v>
       </c>
       <c r="C8" s="6" t="e">
         <v>#VALUE!</v>
@@ -1928,10 +1931,10 @@
     </row>
     <row r="9" spans="1:5" ht="34.200000000000003" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" s="5" t="s">
         <v>36</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>38</v>
       </c>
       <c r="C9" s="6" t="e">
         <v>#VALUE!</v>
@@ -1945,10 +1948,10 @@
     </row>
     <row r="10" spans="1:5" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C10" s="6" t="e">
         <v>#VALUE!</v>
@@ -1962,10 +1965,10 @@
     </row>
     <row r="11" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B11" s="5" t="s">
         <v>44</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>46</v>
       </c>
       <c r="C11" s="6" t="e">
         <v>#VALUE!</v>
@@ -1979,10 +1982,10 @@
     </row>
     <row r="12" spans="1:5" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B12" s="5" t="s">
         <v>48</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>50</v>
       </c>
       <c r="C12" s="6" t="e">
         <v>#VALUE!</v>
@@ -1996,10 +1999,10 @@
     </row>
     <row r="13" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C13" s="6" t="e">
         <v>#VALUE!</v>

</xml_diff>